<commit_message>
first import and excel
</commit_message>
<xml_diff>
--- a/tipseur_twitter_id.xlsx
+++ b/tipseur_twitter_id.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Tipseur</t>
   </si>
@@ -49,9 +49,6 @@
     <t>NTK_pronos</t>
   </si>
   <si>
-    <t>Bozoh pass</t>
-  </si>
-  <si>
     <t>bozohPronos</t>
   </si>
   <si>
@@ -82,28 +79,19 @@
     <t>Pronosaurus</t>
   </si>
   <si>
-    <t>@ possible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Winamax from:ValueBet3 -is:retweet -is:reply </t>
+    <t xml:space="preserve">Buteurs from:ValueBet3 -is:retweet -is:reply </t>
   </si>
   <si>
     <t>prend from:ValueBet3 -is:retweet -is:reply</t>
   </si>
   <si>
-    <t>un pourcentage, @ et |</t>
-  </si>
-  <si>
-    <t>a voir …..</t>
+    <t>has:images has:hashtags -✅ from:Tyldumia -is:reply -is:retweet</t>
   </si>
   <si>
     <t>Confiance from:ntkpronos -is:retweet -is:reply</t>
   </si>
   <si>
-    <t>"Book ou match" from:BozohPassFree</t>
-  </si>
-  <si>
-    <t>mise ou match from BozohPronos  -is:retweet -is:reply</t>
+    <t>"si tu suis" from:BozohPronos -is:reply -is:retweet</t>
   </si>
   <si>
     <t>buteur</t>
@@ -119,9 +107,6 @@
   </si>
   <si>
     <t>Football mais bcp de screen avec des tips solo</t>
-  </si>
-  <si>
-    <t>Pass payant foot</t>
   </si>
   <si>
     <t xml:space="preserve">Football et montante </t>
@@ -540,13 +525,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2">
-        <v>1.56144214547048e+18</v>
+        <v>1.561437435409613e+18</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -557,13 +542,13 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3">
         <v>1.56141924663024e+18</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -574,13 +559,13 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1.561428521993503e+18</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -590,14 +575,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -608,33 +590,30 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>1.561413432972288e+18</v>
+        <v>1.561428580210512e+18</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1.561301884983542e+18</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -644,14 +623,11 @@
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -665,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -679,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -693,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -707,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -721,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -735,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -749,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -759,17 +735,8 @@
       <c r="D16">
         <v>15</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="17" spans="4:4">
       <c r="D17">
         <v>16</v>
       </c>

</xml_diff>